<commit_message>
Added Null Object, Strategy, and Factory design patterns to the model.events package. Made a minor (< 1 line) modification to MapScreenController to accomadate this change.  Updated the extra credit sheet accordingly.
</commit_message>
<xml_diff>
--- a/artifacts/extra_credit.xlsx
+++ b/artifacts/extra_credit.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="396" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="269" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Total Points</t>
   </si>
@@ -57,6 +57,18 @@
   </si>
   <si>
     <t>Additional gadgets for the ship (Fuel Gadget, Cloaking, Cargo)</t>
+  </si>
+  <si>
+    <t>Factory Method in model.events.EventFactory</t>
+  </si>
+  <si>
+    <t>[assumed]</t>
+  </si>
+  <si>
+    <t>Strategy Pattern for creating RandomEvents (model.events)</t>
+  </si>
+  <si>
+    <t>Null Object pattern for creating EventStrategy in model.events</t>
   </si>
 </sst>
 </file>
@@ -71,6 +83,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -92,6 +105,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -160,13 +174,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:D9"/>
+  <dimension ref="A2:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -193,7 +207,7 @@
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <f aca="false">SUM(B3:B30)</f>
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>5</v>
@@ -257,6 +271,36 @@
       </c>
       <c r="D9" s="0" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>